<commit_message>
Update absence with right cumulative data
</commit_message>
<xml_diff>
--- a/data/C1718.xlsx
+++ b/data/C1718.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="307">
   <si>
     <t>grupo</t>
   </si>
@@ -48,445 +48,877 @@
     <t>ESO</t>
   </si>
   <si>
+    <t>3.49</t>
+  </si>
+  <si>
+    <t>5.48</t>
+  </si>
+  <si>
     <t>ESO1B</t>
   </si>
   <si>
+    <t>2.41</t>
+  </si>
+  <si>
+    <t>3.77</t>
+  </si>
+  <si>
     <t>ESO1C</t>
   </si>
   <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>4.22</t>
+  </si>
+  <si>
     <t>ESO1D</t>
   </si>
   <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>2.58</t>
+  </si>
+  <si>
     <t>ESO2A</t>
   </si>
   <si>
+    <t>1.54</t>
+  </si>
+  <si>
+    <t>4.52</t>
+  </si>
+  <si>
     <t>ESO2B</t>
   </si>
   <si>
+    <t>1.96</t>
+  </si>
+  <si>
+    <t>3.36</t>
+  </si>
+  <si>
     <t>ESO2C</t>
   </si>
   <si>
+    <t>0.20</t>
+  </si>
+  <si>
+    <t>3.27</t>
+  </si>
+  <si>
     <t>ESO2Z</t>
   </si>
   <si>
+    <t>1.66</t>
+  </si>
+  <si>
+    <t>9.31</t>
+  </si>
+  <si>
     <t>ESO3A</t>
   </si>
   <si>
+    <t>3.94</t>
+  </si>
+  <si>
+    <t>4.90</t>
+  </si>
+  <si>
     <t>ESO3B</t>
   </si>
   <si>
+    <t>2.62</t>
+  </si>
+  <si>
+    <t>4.36</t>
+  </si>
+  <si>
     <t>ESO3Z</t>
   </si>
   <si>
+    <t>3.12</t>
+  </si>
+  <si>
+    <t>13.11</t>
+  </si>
+  <si>
     <t>ESO4A</t>
   </si>
   <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>3.01</t>
+  </si>
+  <si>
     <t>ESO4B</t>
   </si>
   <si>
+    <t>2.59</t>
+  </si>
+  <si>
+    <t>2.84</t>
+  </si>
+  <si>
     <t>1FPB</t>
   </si>
   <si>
     <t>FPB</t>
   </si>
   <si>
+    <t>2.45</t>
+  </si>
+  <si>
+    <t>40.25</t>
+  </si>
+  <si>
     <t>2FPB</t>
   </si>
   <si>
+    <t>3.90</t>
+  </si>
+  <si>
+    <t>8.44</t>
+  </si>
+  <si>
     <t>1CIE</t>
   </si>
   <si>
     <t>BACH</t>
   </si>
   <si>
+    <t>4.00</t>
+  </si>
+  <si>
+    <t>1.71</t>
+  </si>
+  <si>
     <t>1SOC</t>
   </si>
   <si>
+    <t>1.36</t>
+  </si>
+  <si>
+    <t>3.15</t>
+  </si>
+  <si>
     <t>2CIE</t>
   </si>
   <si>
+    <t>2.23</t>
+  </si>
+  <si>
+    <t>4.18</t>
+  </si>
+  <si>
     <t>2SOC</t>
   </si>
   <si>
+    <t>1.68</t>
+  </si>
+  <si>
+    <t>2.93</t>
+  </si>
+  <si>
     <t>1TEL</t>
   </si>
   <si>
     <t>CFGM</t>
   </si>
   <si>
+    <t>4.23</t>
+  </si>
+  <si>
+    <t>10.47</t>
+  </si>
+  <si>
     <t>1ELE</t>
   </si>
   <si>
+    <t>4.01</t>
+  </si>
+  <si>
+    <t>16.70</t>
+  </si>
+  <si>
     <t>1CAR</t>
   </si>
   <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>29.24</t>
+  </si>
+  <si>
     <t>2TEL</t>
   </si>
   <si>
+    <t>1.72</t>
+  </si>
+  <si>
+    <t>5.73</t>
+  </si>
+  <si>
     <t>2ELE</t>
   </si>
   <si>
+    <t>2.57</t>
+  </si>
+  <si>
+    <t>5.38</t>
+  </si>
+  <si>
     <t>2CAR</t>
   </si>
   <si>
+    <t>0.32</t>
+  </si>
+  <si>
+    <t>8.75</t>
+  </si>
+  <si>
     <t>1ARI</t>
   </si>
   <si>
     <t>CFGS</t>
   </si>
   <si>
+    <t>3.05</t>
+  </si>
+  <si>
+    <t>10.12</t>
+  </si>
+  <si>
     <t>1ALO</t>
   </si>
   <si>
+    <t>0.56</t>
+  </si>
+  <si>
+    <t>13.84</t>
+  </si>
+  <si>
     <t>1GIT</t>
   </si>
   <si>
+    <t>3.78</t>
+  </si>
+  <si>
+    <t>10.55</t>
+  </si>
+  <si>
     <t>1ASR</t>
   </si>
   <si>
+    <t>3.69</t>
+  </si>
+  <si>
+    <t>10.61</t>
+  </si>
+  <si>
     <t>1DAW</t>
   </si>
   <si>
+    <t>1.37</t>
+  </si>
+  <si>
+    <t>17.59</t>
+  </si>
+  <si>
     <t>2ARI</t>
   </si>
   <si>
+    <t>1.58</t>
+  </si>
+  <si>
+    <t>5.67</t>
+  </si>
+  <si>
     <t>2ALO</t>
   </si>
   <si>
+    <t>2.95</t>
+  </si>
+  <si>
+    <t>7.37</t>
+  </si>
+  <si>
     <t>2GIT</t>
   </si>
   <si>
+    <t>13.25</t>
+  </si>
+  <si>
     <t>2ASR</t>
   </si>
   <si>
+    <t>1.08</t>
+  </si>
+  <si>
+    <t>3.86</t>
+  </si>
+  <si>
     <t>2DAW</t>
   </si>
   <si>
+    <t>2.05</t>
+  </si>
+  <si>
+    <t>11.46</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>5.75</t>
+  </si>
+  <si>
+    <t>0.41</t>
+  </si>
+  <si>
+    <t>6.88</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>1.45</t>
+  </si>
+  <si>
     <t>24.00</t>
   </si>
   <si>
+    <t>5.47</t>
+  </si>
+  <si>
     <t>31.80</t>
   </si>
   <si>
+    <t>2.40</t>
+  </si>
+  <si>
     <t>40.00</t>
   </si>
   <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>5.10</t>
+  </si>
+  <si>
     <t>37.00</t>
   </si>
   <si>
+    <t>0.82</t>
+  </si>
+  <si>
+    <t>3.51</t>
+  </si>
+  <si>
     <t>37.90</t>
   </si>
   <si>
+    <t>3.18</t>
+  </si>
+  <si>
+    <t>5.05</t>
+  </si>
+  <si>
     <t>34.50</t>
   </si>
   <si>
+    <t>3.83</t>
+  </si>
+  <si>
     <t>44.40</t>
   </si>
   <si>
+    <t>0.33</t>
+  </si>
+  <si>
+    <t>4.40</t>
+  </si>
+  <si>
     <t>7.70</t>
   </si>
   <si>
+    <t>3.28</t>
+  </si>
+  <si>
+    <t>10.95</t>
+  </si>
+  <si>
     <t>25.00</t>
   </si>
   <si>
+    <t>4.10</t>
+  </si>
+  <si>
+    <t>4.77</t>
+  </si>
+  <si>
     <t>11.10</t>
   </si>
   <si>
+    <t>2.83</t>
+  </si>
+  <si>
+    <t>5.24</t>
+  </si>
+  <si>
     <t>15.40</t>
   </si>
   <si>
+    <t>4.38</t>
+  </si>
+  <si>
+    <t>14.31</t>
+  </si>
+  <si>
     <t>35.70</t>
   </si>
   <si>
+    <t>2.33</t>
+  </si>
+  <si>
+    <t>2.81</t>
+  </si>
+  <si>
+    <t>3.45</t>
+  </si>
+  <si>
     <t>18.20</t>
   </si>
   <si>
+    <t>3.70</t>
+  </si>
+  <si>
+    <t>34.63</t>
+  </si>
+  <si>
     <t>63.60</t>
   </si>
   <si>
+    <t>4.13</t>
+  </si>
+  <si>
+    <t>8.34</t>
+  </si>
+  <si>
     <t>26.10</t>
   </si>
   <si>
+    <t>4.99</t>
+  </si>
+  <si>
+    <t>2.17</t>
+  </si>
+  <si>
     <t>50.00</t>
   </si>
   <si>
+    <t>2.32</t>
+  </si>
+  <si>
+    <t>3.33</t>
+  </si>
+  <si>
     <t>60.00</t>
   </si>
   <si>
+    <t>2.91</t>
+  </si>
+  <si>
     <t>47.60</t>
   </si>
   <si>
+    <t>1.97</t>
+  </si>
+  <si>
+    <t>3.53</t>
+  </si>
+  <si>
     <t>17.60</t>
   </si>
   <si>
+    <t>5.20</t>
+  </si>
+  <si>
+    <t>9.16</t>
+  </si>
+  <si>
     <t>21.40</t>
   </si>
   <si>
+    <t>19.04</t>
+  </si>
+  <si>
     <t>47.40</t>
   </si>
   <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>28.69</t>
+  </si>
+  <si>
     <t>100.00</t>
   </si>
   <si>
+    <t>1.51</t>
+  </si>
+  <si>
+    <t>4.86</t>
+  </si>
+  <si>
     <t>88.90</t>
   </si>
   <si>
+    <t>1.78</t>
+  </si>
+  <si>
+    <t>4.88</t>
+  </si>
+  <si>
     <t>90.90</t>
   </si>
   <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>10.69</t>
+  </si>
+  <si>
     <t>41.20</t>
   </si>
   <si>
+    <t>8.62</t>
+  </si>
+  <si>
     <t>75.90</t>
   </si>
   <si>
+    <t>1.41</t>
+  </si>
+  <si>
+    <t>13.00</t>
+  </si>
+  <si>
+    <t>11.06</t>
+  </si>
+  <si>
     <t>41.70</t>
   </si>
   <si>
+    <t>10.27</t>
+  </si>
+  <si>
     <t>38.10</t>
   </si>
   <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>20.18</t>
+  </si>
+  <si>
+    <t>1.03</t>
+  </si>
+  <si>
+    <t>4.54</t>
+  </si>
+  <si>
     <t>95.50</t>
   </si>
   <si>
+    <t>2.72</t>
+  </si>
+  <si>
+    <t>5.55</t>
+  </si>
+  <si>
     <t>82.40</t>
   </si>
   <si>
+    <t>12.59</t>
+  </si>
+  <si>
     <t>94.70</t>
   </si>
   <si>
+    <t>1.22</t>
+  </si>
+  <si>
+    <t>4.72</t>
+  </si>
+  <si>
     <t>71.40</t>
   </si>
   <si>
+    <t>9.87</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>6.78</t>
+  </si>
+  <si>
+    <t>0.24</t>
+  </si>
+  <si>
+    <t>6.19</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>2.36</t>
+  </si>
+  <si>
+    <t>5.61</t>
+  </si>
+  <si>
+    <t>45.50</t>
+  </si>
+  <si>
+    <t>2.54</t>
+  </si>
+  <si>
+    <t>2.67</t>
+  </si>
+  <si>
+    <t>52.00</t>
+  </si>
+  <si>
+    <t>1.57</t>
+  </si>
+  <si>
+    <t>5.35</t>
+  </si>
+  <si>
+    <t>55.60</t>
+  </si>
+  <si>
+    <t>1.27</t>
+  </si>
+  <si>
+    <t>4.20</t>
+  </si>
+  <si>
+    <t>55.20</t>
+  </si>
+  <si>
+    <t>3.19</t>
+  </si>
+  <si>
+    <t>48.30</t>
+  </si>
+  <si>
+    <t>2.43</t>
+  </si>
+  <si>
+    <t>3.92</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>3.72</t>
+  </si>
+  <si>
+    <t>3.41</t>
+  </si>
+  <si>
+    <t>14.00</t>
+  </si>
+  <si>
+    <t>42.90</t>
+  </si>
+  <si>
+    <t>3.67</t>
+  </si>
+  <si>
+    <t>4.75</t>
+  </si>
+  <si>
+    <t>22.20</t>
+  </si>
+  <si>
+    <t>6.16</t>
+  </si>
+  <si>
+    <t>9.10</t>
+  </si>
+  <si>
+    <t>4.64</t>
+  </si>
+  <si>
+    <t>14.23</t>
+  </si>
+  <si>
+    <t>39.30</t>
+  </si>
+  <si>
+    <t>1.90</t>
+  </si>
+  <si>
+    <t>32.33</t>
+  </si>
+  <si>
+    <t>3.16</t>
+  </si>
+  <si>
+    <t>6.40</t>
+  </si>
+  <si>
+    <t>43.50</t>
+  </si>
+  <si>
+    <t>2.70</t>
+  </si>
+  <si>
+    <t>65.40</t>
+  </si>
+  <si>
+    <t>2.16</t>
+  </si>
+  <si>
+    <t>2.51</t>
+  </si>
+  <si>
+    <t>88.00</t>
+  </si>
+  <si>
     <t>2.26</t>
   </si>
   <si>
-    <t>5.91</t>
-  </si>
-  <si>
-    <t>45.50</t>
-  </si>
-  <si>
-    <t>2.87</t>
-  </si>
-  <si>
-    <t>1.91</t>
-  </si>
-  <si>
-    <t>52.00</t>
-  </si>
-  <si>
-    <t>2.80</t>
-  </si>
-  <si>
-    <t>5.88</t>
-  </si>
-  <si>
-    <t>55.60</t>
-  </si>
-  <si>
-    <t>2.23</t>
-  </si>
-  <si>
-    <t>5.64</t>
-  </si>
-  <si>
-    <t>55.20</t>
-  </si>
-  <si>
-    <t>3.20</t>
-  </si>
-  <si>
-    <t>4.45</t>
-  </si>
-  <si>
-    <t>48.30</t>
-  </si>
-  <si>
-    <t>2.49</t>
-  </si>
-  <si>
-    <t>4.09</t>
-  </si>
-  <si>
-    <t>2.09</t>
-  </si>
-  <si>
-    <t>2.27</t>
-  </si>
-  <si>
-    <t>3.71</t>
-  </si>
-  <si>
-    <t>20.92</t>
-  </si>
-  <si>
-    <t>42.90</t>
-  </si>
-  <si>
-    <t>2.73</t>
-  </si>
-  <si>
-    <t>4.71</t>
-  </si>
-  <si>
-    <t>22.20</t>
-  </si>
-  <si>
-    <t>1.24</t>
-  </si>
-  <si>
-    <t>8.14</t>
-  </si>
-  <si>
-    <t>9.10</t>
-  </si>
-  <si>
-    <t>5.32</t>
-  </si>
-  <si>
-    <t>14.02</t>
-  </si>
-  <si>
-    <t>39.30</t>
-  </si>
-  <si>
-    <t>0.98</t>
-  </si>
-  <si>
-    <t>3.88</t>
-  </si>
-  <si>
-    <t>3.01</t>
-  </si>
-  <si>
-    <t>2.90</t>
-  </si>
-  <si>
-    <t>3.00</t>
-  </si>
-  <si>
-    <t>25.35</t>
-  </si>
-  <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>1.87</t>
-  </si>
-  <si>
-    <t>43.50</t>
-  </si>
-  <si>
-    <t>3.89</t>
+    <t>66.70</t>
+  </si>
+  <si>
+    <t>1.44</t>
+  </si>
+  <si>
+    <t>3.03</t>
+  </si>
+  <si>
+    <t>58.80</t>
+  </si>
+  <si>
+    <t>10.08</t>
+  </si>
+  <si>
+    <t>38.50</t>
+  </si>
+  <si>
+    <t>3.64</t>
+  </si>
+  <si>
+    <t>21.73</t>
+  </si>
+  <si>
+    <t>61.50</t>
+  </si>
+  <si>
+    <t>0.53</t>
+  </si>
+  <si>
+    <t>31.23</t>
+  </si>
+  <si>
+    <t>1.19</t>
   </si>
   <si>
     <t>3.84</t>
   </si>
   <si>
-    <t>65.40</t>
-  </si>
-  <si>
-    <t>1.82</t>
-  </si>
-  <si>
-    <t>0.69</t>
-  </si>
-  <si>
-    <t>88.00</t>
-  </si>
-  <si>
-    <t>0.78</t>
-  </si>
-  <si>
-    <t>3.19</t>
-  </si>
-  <si>
-    <t>66.70</t>
-  </si>
-  <si>
-    <t>0.31</t>
-  </si>
-  <si>
-    <t>1.96</t>
-  </si>
-  <si>
-    <t>58.80</t>
-  </si>
-  <si>
-    <t>1.41</t>
-  </si>
-  <si>
-    <t>12.09</t>
-  </si>
-  <si>
-    <t>38.50</t>
-  </si>
-  <si>
-    <t>3.31</t>
-  </si>
-  <si>
-    <t>28.28</t>
-  </si>
-  <si>
-    <t>61.50</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>37.49</t>
+    <t>1.59</t>
+  </si>
+  <si>
+    <t>4.34</t>
+  </si>
+  <si>
+    <t>8.78</t>
   </si>
   <si>
     <t>70.60</t>
   </si>
   <si>
-    <t>2.03</t>
-  </si>
-  <si>
-    <t>6.00</t>
+    <t>7.80</t>
   </si>
   <si>
     <t>78.60</t>
   </si>
   <si>
-    <t>0.47</t>
-  </si>
-  <si>
-    <t>9.65</t>
+    <t>1.12</t>
+  </si>
+  <si>
+    <t>11.96</t>
   </si>
   <si>
     <t>62.10</t>
   </si>
   <si>
-    <t>1.83</t>
-  </si>
-  <si>
-    <t>7.07</t>
-  </si>
-  <si>
-    <t>6.25</t>
+    <t>4.02</t>
+  </si>
+  <si>
+    <t>9.79</t>
+  </si>
+  <si>
+    <t>3.35</t>
+  </si>
+  <si>
+    <t>9.11</t>
   </si>
   <si>
     <t>61.10</t>
   </si>
   <si>
-    <t>0.95</t>
-  </si>
-  <si>
-    <t>23.56</t>
+    <t>1.07</t>
+  </si>
+  <si>
+    <t>21.04</t>
+  </si>
+  <si>
+    <t>0.83</t>
   </si>
   <si>
     <t>90.50</t>
   </si>
   <si>
+    <t>2.14</t>
+  </si>
+  <si>
+    <t>4.37</t>
+  </si>
+  <si>
+    <t>3.59</t>
+  </si>
+  <si>
+    <t>10.01</t>
+  </si>
+  <si>
+    <t>1.04</t>
+  </si>
+  <si>
+    <t>4.03</t>
+  </si>
+  <si>
+    <t>1.13</t>
+  </si>
+  <si>
+    <t>8.13</t>
+  </si>
+  <si>
     <t>1DAM</t>
   </si>
   <si>
     <t>18.60</t>
   </si>
   <si>
-    <t>3.08</t>
+    <t>5.62</t>
   </si>
   <si>
     <t>2DAM</t>
@@ -495,10 +927,16 @@
     <t>42.10</t>
   </si>
   <si>
-    <t>10.45</t>
+    <t>0.17</t>
+  </si>
+  <si>
+    <t>7.57</t>
   </si>
   <si>
     <t>3DAM</t>
+  </si>
+  <si>
+    <t>0.61</t>
   </si>
 </sst>
 </file>
@@ -821,7 +1259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90">
       <selection activeCell="B15" sqref="B15"/>
@@ -869,13 +1307,11 @@
       <c r="C2" t="n">
         <v>32</v>
       </c>
-      <c r="D2">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E2">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
@@ -886,7 +1322,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -894,13 +1330,11 @@
       <c r="C3" t="n">
         <v>43.5</v>
       </c>
-      <c r="D3">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E3">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
       </c>
       <c r="H3" t="n">
         <v>22</v>
@@ -908,7 +1342,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -916,13 +1350,11 @@
       <c r="C4" t="n">
         <v>44</v>
       </c>
-      <c r="D4">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E4">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
       </c>
       <c r="F4" t="n">
         <v>3</v>
@@ -933,7 +1365,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -941,13 +1373,11 @@
       <c r="C5" t="n">
         <v>46.2</v>
       </c>
-      <c r="D5">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E5">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
@@ -958,7 +1388,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -966,13 +1396,11 @@
       <c r="C6" t="n">
         <v>24.1</v>
       </c>
-      <c r="D6">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E6">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
       </c>
       <c r="F6" t="n">
         <v>10</v>
@@ -986,7 +1414,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -994,13 +1422,11 @@
       <c r="C7" t="n">
         <v>34.5</v>
       </c>
-      <c r="D7">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E7">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
       </c>
       <c r="F7" t="n">
         <v>16</v>
@@ -1014,7 +1440,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -1022,13 +1448,11 @@
       <c r="C8" t="n">
         <v>44.4</v>
       </c>
-      <c r="D8">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E8">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
       </c>
       <c r="H8" t="n">
         <v>18</v>
@@ -1036,7 +1460,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -1044,13 +1468,11 @@
       <c r="C9" t="n">
         <v>7.7</v>
       </c>
-      <c r="D9">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E9">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
       </c>
       <c r="F9" t="n">
         <v>4</v>
@@ -1061,7 +1483,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -1069,13 +1491,11 @@
       <c r="C10" t="n">
         <v>20.7</v>
       </c>
-      <c r="D10">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E10">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
       </c>
       <c r="F10" t="n">
         <v>3</v>
@@ -1086,7 +1506,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -1094,13 +1514,11 @@
       <c r="C11" t="n">
         <v>3.6</v>
       </c>
-      <c r="D11">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E11">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
       </c>
       <c r="F11" t="n">
         <v>8</v>
@@ -1111,7 +1529,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1119,13 +1537,11 @@
       <c r="C12" t="n">
         <v>6.7</v>
       </c>
-      <c r="D12">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E12">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
       </c>
       <c r="F12" t="n">
         <v>15</v>
@@ -1136,7 +1552,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -1144,13 +1560,11 @@
       <c r="C13" t="n">
         <v>25.9</v>
       </c>
-      <c r="D13">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E13">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
       </c>
       <c r="H13" t="n">
         <v>28</v>
@@ -1158,7 +1572,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -1166,13 +1580,11 @@
       <c r="C14" t="n">
         <v>32</v>
       </c>
-      <c r="D14">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E14">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
       </c>
       <c r="H14" t="n">
         <v>26</v>
@@ -1180,21 +1592,19 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C15" t="n">
         <v>11.1</v>
       </c>
-      <c r="D15">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E15">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
       </c>
       <c r="F15" t="n">
         <v>16</v>
@@ -1208,21 +1618,19 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C16" t="n">
         <v>63.6</v>
       </c>
-      <c r="D16">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E16">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>54</v>
       </c>
       <c r="F16" t="n">
         <v>1</v>
@@ -1233,21 +1641,19 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C17" t="n">
         <v>47.8</v>
       </c>
-      <c r="D17">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E17">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
       </c>
       <c r="H17" t="n">
         <v>23</v>
@@ -1255,21 +1661,19 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C18" t="n">
         <v>48.1</v>
       </c>
-      <c r="D18">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E18">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
@@ -1280,21 +1684,19 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C19" t="n">
         <v>51.9</v>
       </c>
-      <c r="D19">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E19">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
       </c>
       <c r="H19" t="n">
         <v>27</v>
@@ -1302,21 +1704,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C20" t="n">
         <v>38.1</v>
       </c>
-      <c r="D20">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E20">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
       </c>
       <c r="H20" t="n">
         <v>21</v>
@@ -1324,21 +1724,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C21" t="n">
         <v>29.4</v>
       </c>
-      <c r="D21">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E21">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
       </c>
       <c r="F21" t="n">
         <v>1</v>
@@ -1352,21 +1750,19 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C22" t="n">
         <v>6.2</v>
       </c>
-      <c r="D22">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E22">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
       </c>
       <c r="H22" t="n">
         <v>14</v>
@@ -1374,21 +1770,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C23" t="n">
         <v>55</v>
       </c>
-      <c r="D23">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E23">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>77</v>
       </c>
       <c r="F23" t="n">
         <v>2</v>
@@ -1399,21 +1793,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C24" t="n">
         <v>90.90000000000001</v>
       </c>
-      <c r="D24">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E24">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" t="s">
+        <v>80</v>
       </c>
       <c r="H24" t="n">
         <v>11</v>
@@ -1421,21 +1813,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C25" t="n">
         <v>66.7</v>
       </c>
-      <c r="D25">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E25">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" t="s">
+        <v>83</v>
       </c>
       <c r="H25" t="n">
         <v>9</v>
@@ -1443,21 +1833,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C26" t="n">
         <v>81.8</v>
       </c>
-      <c r="D26">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E26">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" t="s">
+        <v>86</v>
       </c>
       <c r="H26" t="n">
         <v>11</v>
@@ -1465,21 +1853,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C27" t="n">
         <v>41.2</v>
       </c>
-      <c r="D27">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E27">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" t="s">
+        <v>90</v>
       </c>
       <c r="H27" t="n">
         <v>17</v>
@@ -1487,21 +1873,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C28" t="n">
         <v>65.5</v>
       </c>
-      <c r="D28">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E28">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" t="s">
+        <v>93</v>
       </c>
       <c r="F28" t="n">
         <v>1</v>
@@ -1515,21 +1899,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C29" t="n">
         <v>44.8</v>
       </c>
-      <c r="D29">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E29">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" t="s">
+        <v>96</v>
       </c>
       <c r="H29" t="n">
         <v>29</v>
@@ -1537,21 +1919,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C30" t="n">
         <v>32.1</v>
       </c>
-      <c r="D30">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E30">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" t="s">
+        <v>99</v>
       </c>
       <c r="H30" t="n">
         <v>26</v>
@@ -1559,21 +1939,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C31" t="n">
         <v>15.4</v>
       </c>
-      <c r="D31">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E31">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D31" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" t="s">
+        <v>102</v>
       </c>
       <c r="H31" t="n">
         <v>26</v>
@@ -1581,21 +1959,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C32" t="n">
         <v>45.5</v>
       </c>
-      <c r="D32">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E32">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" t="s">
+        <v>105</v>
       </c>
       <c r="H32" t="n">
         <v>12</v>
@@ -1603,21 +1979,19 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C33" t="n">
         <v>77.3</v>
       </c>
-      <c r="D33">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E33">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D33" t="s">
+        <v>107</v>
+      </c>
+      <c r="E33" t="s">
+        <v>108</v>
       </c>
       <c r="H33" t="n">
         <v>23</v>
@@ -1625,21 +1999,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C34" t="n">
         <v>72.2</v>
       </c>
-      <c r="D34">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E34">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>110</v>
       </c>
       <c r="H34" t="n">
         <v>19</v>
@@ -1647,21 +2019,19 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C35" t="n">
         <v>94.7</v>
       </c>
-      <c r="D35">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E35">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" t="s">
+        <v>113</v>
       </c>
       <c r="H35" t="n">
         <v>19</v>
@@ -1669,24 +2039,46 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C36" t="n">
         <v>40</v>
       </c>
-      <c r="D36">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E36">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+      <c r="D36" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" t="s">
+        <v>116</v>
       </c>
       <c r="H36" t="n">
         <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="D37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="D38" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="D39" t="s">
+        <v>121</v>
+      </c>
+      <c r="E39" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1700,7 +2092,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -1745,15 +2137,13 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E2">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>124</v>
       </c>
       <c r="F2" t="n">
         <v>3</v>
@@ -1764,21 +2154,19 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E3">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>125</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
       </c>
       <c r="F3" t="n">
         <v>2</v>
@@ -1792,21 +2180,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E4">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>127</v>
+      </c>
+      <c r="D4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
       </c>
       <c r="F4" t="n">
         <v>4</v>
@@ -1817,21 +2203,19 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E5">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>130</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" t="s">
+        <v>132</v>
       </c>
       <c r="F5" t="n">
         <v>5</v>
@@ -1842,21 +2226,19 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E6">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>133</v>
+      </c>
+      <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" t="s">
+        <v>135</v>
       </c>
       <c r="F6" t="n">
         <v>7</v>
@@ -1870,21 +2252,19 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E7">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>136</v>
+      </c>
+      <c r="D7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" t="s">
+        <v>137</v>
       </c>
       <c r="F7" t="n">
         <v>5</v>
@@ -1898,21 +2278,19 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E8">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>138</v>
+      </c>
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" t="s">
+        <v>140</v>
       </c>
       <c r="F8" t="n">
         <v>3</v>
@@ -1923,21 +2301,19 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E9">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>141</v>
+      </c>
+      <c r="D9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" t="s">
+        <v>143</v>
       </c>
       <c r="F9" t="n">
         <v>13</v>
@@ -1951,21 +2327,19 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E10">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>144</v>
+      </c>
+      <c r="D10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" t="s">
+        <v>146</v>
       </c>
       <c r="F10" t="n">
         <v>16</v>
@@ -1979,21 +2353,19 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E11">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>147</v>
+      </c>
+      <c r="D11" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" t="s">
+        <v>149</v>
       </c>
       <c r="F11" t="n">
         <v>4</v>
@@ -2004,21 +2376,19 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E12">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>150</v>
+      </c>
+      <c r="D12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" t="s">
+        <v>152</v>
       </c>
       <c r="F12" t="n">
         <v>11</v>
@@ -2032,21 +2402,19 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E13">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>153</v>
+      </c>
+      <c r="D13" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" t="s">
+        <v>155</v>
       </c>
       <c r="H13" t="n">
         <v>28</v>
@@ -2054,21 +2422,19 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E14">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>123</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>156</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -2079,21 +2445,19 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E15">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>157</v>
+      </c>
+      <c r="D15" t="s">
+        <v>158</v>
+      </c>
+      <c r="E15" t="s">
+        <v>159</v>
       </c>
       <c r="F15" t="n">
         <v>11</v>
@@ -2107,21 +2471,19 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E16">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>160</v>
+      </c>
+      <c r="D16" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" t="s">
+        <v>162</v>
       </c>
       <c r="H16" t="n">
         <v>11</v>
@@ -2129,21 +2491,19 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E17">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>163</v>
+      </c>
+      <c r="D17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E17" t="s">
+        <v>165</v>
       </c>
       <c r="H17" t="n">
         <v>23</v>
@@ -2151,21 +2511,19 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E18">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>166</v>
+      </c>
+      <c r="D18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E18" t="s">
+        <v>168</v>
       </c>
       <c r="H18" t="n">
         <v>26</v>
@@ -2173,21 +2531,19 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E19">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>169</v>
+      </c>
+      <c r="D19" t="s">
+        <v>170</v>
+      </c>
+      <c r="E19" t="s">
+        <v>129</v>
       </c>
       <c r="H19" t="n">
         <v>25</v>
@@ -2195,21 +2551,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E20">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>171</v>
+      </c>
+      <c r="D20" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20" t="s">
+        <v>173</v>
       </c>
       <c r="H20" t="n">
         <v>21</v>
@@ -2217,21 +2571,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E21">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>174</v>
+      </c>
+      <c r="D21" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" t="s">
+        <v>176</v>
       </c>
       <c r="F21" t="n">
         <v>1</v>
@@ -2242,21 +2594,19 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E22">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>177</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>178</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
@@ -2267,21 +2617,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E23">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>179</v>
+      </c>
+      <c r="D23" t="s">
+        <v>180</v>
+      </c>
+      <c r="E23" t="s">
+        <v>181</v>
       </c>
       <c r="F23" t="n">
         <v>1</v>
@@ -2292,21 +2640,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E24">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>182</v>
+      </c>
+      <c r="D24" t="s">
+        <v>183</v>
+      </c>
+      <c r="E24" t="s">
+        <v>184</v>
       </c>
       <c r="H24" t="n">
         <v>11</v>
@@ -2314,21 +2660,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E25">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>185</v>
+      </c>
+      <c r="D25" t="s">
+        <v>186</v>
+      </c>
+      <c r="E25" t="s">
+        <v>187</v>
       </c>
       <c r="H25" t="n">
         <v>9</v>
@@ -2336,21 +2680,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E26">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>188</v>
+      </c>
+      <c r="D26" t="s">
+        <v>189</v>
+      </c>
+      <c r="E26" t="s">
+        <v>190</v>
       </c>
       <c r="H26" t="n">
         <v>11</v>
@@ -2358,21 +2700,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E27">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>191</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>192</v>
       </c>
       <c r="H27" t="n">
         <v>17</v>
@@ -2380,21 +2720,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E28">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>193</v>
+      </c>
+      <c r="D28" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" t="s">
+        <v>195</v>
       </c>
       <c r="H28" t="n">
         <v>29</v>
@@ -2402,21 +2740,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E29">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>136</v>
+      </c>
+      <c r="D29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" t="s">
+        <v>196</v>
       </c>
       <c r="H29" t="n">
         <v>29</v>
@@ -2424,21 +2760,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E30">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>197</v>
+      </c>
+      <c r="D30" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" t="s">
+        <v>198</v>
       </c>
       <c r="H30" t="n">
         <v>24</v>
@@ -2446,21 +2780,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E31">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>199</v>
+      </c>
+      <c r="D31" t="s">
+        <v>200</v>
+      </c>
+      <c r="E31" t="s">
+        <v>201</v>
       </c>
       <c r="H31" t="n">
         <v>21</v>
@@ -2468,21 +2800,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E32">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>188</v>
+      </c>
+      <c r="D32" t="s">
+        <v>202</v>
+      </c>
+      <c r="E32" t="s">
+        <v>203</v>
       </c>
       <c r="H32" t="n">
         <v>11</v>
@@ -2490,21 +2820,19 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E33">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>204</v>
+      </c>
+      <c r="D33" t="s">
+        <v>205</v>
+      </c>
+      <c r="E33" t="s">
+        <v>206</v>
       </c>
       <c r="H33" t="n">
         <v>22</v>
@@ -2512,21 +2840,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E34">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>207</v>
+      </c>
+      <c r="D34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" t="s">
+        <v>208</v>
       </c>
       <c r="H34" t="n">
         <v>17</v>
@@ -2534,21 +2860,19 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E35">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>209</v>
+      </c>
+      <c r="D35" t="s">
+        <v>210</v>
+      </c>
+      <c r="E35" t="s">
+        <v>211</v>
       </c>
       <c r="H35" t="n">
         <v>19</v>
@@ -2556,24 +2880,46 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
-      </c>
-      <c r="E36">
-        <f>RANDBETWEEN(0, 25)</f>
-        <v/>
+        <v>212</v>
+      </c>
+      <c r="D36" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" t="s">
+        <v>213</v>
       </c>
       <c r="H36" t="n">
         <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="D37" t="s">
+        <v>214</v>
+      </c>
+      <c r="E37" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="D38" t="s">
+        <v>216</v>
+      </c>
+      <c r="E38" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="D39" t="s">
+        <v>121</v>
+      </c>
+      <c r="E39" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2629,13 +2975,13 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>166</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>219</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>220</v>
       </c>
       <c r="F2" t="n">
         <v>2</v>
@@ -2649,19 +2995,19 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>221</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>222</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>223</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -2672,19 +3018,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>224</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>225</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>226</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -2695,19 +3041,19 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>227</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>228</v>
       </c>
       <c r="E5" t="s">
-        <v>90</v>
+        <v>229</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
@@ -2721,19 +3067,19 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>230</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>231</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>184</v>
       </c>
       <c r="F6" t="n">
         <v>2</v>
@@ -2747,19 +3093,19 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>232</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>233</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>234</v>
       </c>
       <c r="F7" t="n">
         <v>5</v>
@@ -2773,19 +3119,19 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>166</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>235</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>236</v>
       </c>
       <c r="H8" t="n">
         <v>18</v>
@@ -2793,19 +3139,19 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>237</v>
       </c>
       <c r="E9" t="s">
-        <v>100</v>
+        <v>238</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -2816,19 +3162,19 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>239</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>240</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>241</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -2839,19 +3185,19 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>242</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="E11" t="s">
-        <v>106</v>
+        <v>243</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
@@ -2862,19 +3208,19 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>244</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>245</v>
       </c>
       <c r="E12" t="s">
-        <v>109</v>
+        <v>246</v>
       </c>
       <c r="F12" t="n">
         <v>3</v>
@@ -2885,19 +3231,19 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>247</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="E13" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="H13" t="n">
         <v>28</v>
@@ -2905,19 +3251,19 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>224</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>173</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
+        <v>142</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -2928,19 +3274,19 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>221</v>
       </c>
       <c r="D15" t="s">
-        <v>115</v>
+        <v>173</v>
       </c>
       <c r="E15" t="s">
-        <v>116</v>
+        <v>249</v>
       </c>
       <c r="F15" t="n">
         <v>6</v>
@@ -2954,19 +3300,19 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="D16" t="s">
-        <v>117</v>
+        <v>250</v>
       </c>
       <c r="E16" t="s">
-        <v>118</v>
+        <v>251</v>
       </c>
       <c r="H16" t="n">
         <v>10</v>
@@ -2974,19 +3320,19 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>252</v>
       </c>
       <c r="D17" t="s">
-        <v>120</v>
+        <v>245</v>
       </c>
       <c r="E17" t="s">
-        <v>121</v>
+        <v>253</v>
       </c>
       <c r="H17" t="n">
         <v>23</v>
@@ -2994,19 +3340,19 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>254</v>
       </c>
       <c r="D18" t="s">
-        <v>123</v>
+        <v>255</v>
       </c>
       <c r="E18" t="s">
-        <v>124</v>
+        <v>256</v>
       </c>
       <c r="H18" t="n">
         <v>26</v>
@@ -3014,19 +3360,19 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>257</v>
       </c>
       <c r="D19" t="s">
-        <v>126</v>
+        <v>258</v>
       </c>
       <c r="E19" t="s">
-        <v>127</v>
+        <v>23</v>
       </c>
       <c r="H19" t="n">
         <v>25</v>
@@ -3034,19 +3380,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>128</v>
+        <v>259</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>260</v>
       </c>
       <c r="E20" t="s">
-        <v>130</v>
+        <v>261</v>
       </c>
       <c r="H20" t="n">
         <v>21</v>
@@ -3054,19 +3400,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>262</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>133</v>
+        <v>263</v>
       </c>
       <c r="H21" t="n">
         <v>17</v>
@@ -3074,19 +3420,19 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>134</v>
+        <v>264</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>265</v>
       </c>
       <c r="E22" t="s">
-        <v>136</v>
+        <v>266</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
@@ -3097,19 +3443,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
+        <v>267</v>
       </c>
       <c r="D23" t="s">
-        <v>138</v>
+        <v>268</v>
       </c>
       <c r="E23" t="s">
-        <v>139</v>
+        <v>269</v>
       </c>
       <c r="F23" t="n">
         <v>1</v>
@@ -3120,19 +3466,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="D24" t="s">
-        <v>138</v>
+        <v>270</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
+        <v>271</v>
       </c>
       <c r="H24" t="n">
         <v>11</v>
@@ -3140,19 +3486,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="D25" t="s">
-        <v>138</v>
+        <v>272</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
+        <v>273</v>
       </c>
       <c r="H25" t="n">
         <v>9</v>
@@ -3160,19 +3506,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="D26" t="s">
-        <v>138</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>138</v>
+        <v>274</v>
       </c>
       <c r="H26" t="n">
         <v>10</v>
@@ -3180,19 +3526,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>140</v>
+        <v>275</v>
       </c>
       <c r="D27" t="s">
-        <v>141</v>
+        <v>261</v>
       </c>
       <c r="E27" t="s">
-        <v>142</v>
+        <v>276</v>
       </c>
       <c r="H27" t="n">
         <v>17</v>
@@ -3200,19 +3546,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>143</v>
+        <v>277</v>
       </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>278</v>
       </c>
       <c r="E28" t="s">
-        <v>145</v>
+        <v>279</v>
       </c>
       <c r="H28" t="n">
         <v>28</v>
@@ -3220,19 +3566,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>146</v>
+        <v>280</v>
       </c>
       <c r="D29" t="s">
-        <v>147</v>
+        <v>281</v>
       </c>
       <c r="E29" t="s">
-        <v>148</v>
+        <v>282</v>
       </c>
       <c r="H29" t="n">
         <v>29</v>
@@ -3240,19 +3586,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>197</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>283</v>
       </c>
       <c r="E30" t="s">
-        <v>149</v>
+        <v>284</v>
       </c>
       <c r="H30" t="n">
         <v>24</v>
@@ -3260,19 +3606,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>100</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>285</v>
       </c>
       <c r="D31" t="s">
-        <v>151</v>
+        <v>286</v>
       </c>
       <c r="E31" t="s">
-        <v>152</v>
+        <v>287</v>
       </c>
       <c r="H31" t="n">
         <v>18</v>
@@ -3280,19 +3626,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="D32" t="s">
-        <v>138</v>
+        <v>288</v>
       </c>
       <c r="E32" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="H32" t="n">
         <v>10</v>
@@ -3300,19 +3646,19 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>289</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>290</v>
       </c>
       <c r="E33" t="s">
-        <v>138</v>
+        <v>291</v>
       </c>
       <c r="H33" t="n">
         <v>21</v>
@@ -3320,19 +3666,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="D34" t="s">
-        <v>138</v>
+        <v>292</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
+        <v>293</v>
       </c>
       <c r="H34" t="n">
         <v>15</v>
@@ -3340,19 +3686,19 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="D35" t="s">
-        <v>138</v>
+        <v>294</v>
       </c>
       <c r="E35" t="s">
-        <v>138</v>
+        <v>295</v>
       </c>
       <c r="H35" t="n">
         <v>18</v>
@@ -3360,19 +3706,19 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="D36" t="s">
-        <v>138</v>
+        <v>296</v>
       </c>
       <c r="E36" t="s">
-        <v>138</v>
+        <v>297</v>
       </c>
       <c r="H36" t="n">
         <v>11</v>
@@ -3380,19 +3726,19 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>298</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C37" t="s">
-        <v>155</v>
+        <v>299</v>
       </c>
       <c r="D37" t="s">
-        <v>138</v>
+        <v>214</v>
       </c>
       <c r="E37" t="s">
-        <v>156</v>
+        <v>300</v>
       </c>
       <c r="H37" t="n">
         <v>43</v>
@@ -3400,19 +3746,19 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>301</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C38" t="s">
-        <v>158</v>
+        <v>302</v>
       </c>
       <c r="D38" t="s">
-        <v>138</v>
+        <v>303</v>
       </c>
       <c r="E38" t="s">
-        <v>159</v>
+        <v>304</v>
       </c>
       <c r="H38" t="n">
         <v>19</v>
@@ -3420,19 +3766,19 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>305</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="D39" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>306</v>
       </c>
       <c r="H39" t="n">
         <v>6</v>

</xml_diff>

<commit_message>
Fix Nan values on source files
</commit_message>
<xml_diff>
--- a/data/C1718.xlsx
+++ b/data/C1718.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sdelquin/Dropbox/Code/iespuertodelacruz/analitica/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" tabRatio="500" windowHeight="16500" windowWidth="27740" xWindow="5840" yWindow="3080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="E1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="E2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="E3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="E1" sheetId="1" r:id="rId1"/>
+    <sheet name="E2" sheetId="2" r:id="rId2"/>
+    <sheet name="E3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="150001" concurrentCalc="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="298">
   <si>
     <t>grupo</t>
   </si>
@@ -369,24 +382,9 @@
     <t>11.46</t>
   </si>
   <si>
-    <t>0.04</t>
-  </si>
-  <si>
-    <t>5.75</t>
-  </si>
-  <si>
-    <t>0.41</t>
-  </si>
-  <si>
-    <t>6.88</t>
-  </si>
-  <si>
     <t>0.00</t>
   </si>
   <si>
-    <t>1.45</t>
-  </si>
-  <si>
     <t>24.00</t>
   </si>
   <si>
@@ -661,18 +659,6 @@
   </si>
   <si>
     <t>0.02</t>
-  </si>
-  <si>
-    <t>6.78</t>
-  </si>
-  <si>
-    <t>0.24</t>
-  </si>
-  <si>
-    <t>6.19</t>
-  </si>
-  <si>
-    <t>0.98</t>
   </si>
   <si>
     <t>2.36</t>
@@ -942,28 +928,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -979,16 +964,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1254,24 +1245,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="11.33203125"/>
-    <col customWidth="1" max="7" min="7" width="18.83203125"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:8">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1297,14 +1284,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>32</v>
       </c>
       <c r="D2" t="s">
@@ -1313,21 +1300,21 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>43.5</v>
       </c>
       <c r="D3" t="s">
@@ -1336,18 +1323,18 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>44</v>
       </c>
       <c r="D4" t="s">
@@ -1356,21 +1343,21 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>3</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>46.2</v>
       </c>
       <c r="D5" t="s">
@@ -1379,21 +1366,21 @@
       <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>24.1</v>
       </c>
       <c r="D6" t="s">
@@ -1402,24 +1389,24 @@
       <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>10</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>3</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>34.5</v>
       </c>
       <c r="D7" t="s">
@@ -1428,24 +1415,24 @@
       <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>16</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>3</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>44.4</v>
       </c>
       <c r="D8" t="s">
@@ -1454,18 +1441,18 @@
       <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>7.7</v>
       </c>
       <c r="D9" t="s">
@@ -1474,21 +1461,21 @@
       <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>4</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>20.7</v>
       </c>
       <c r="D10" t="s">
@@ -1497,21 +1484,21 @@
       <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>3</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>3.6</v>
       </c>
       <c r="D11" t="s">
@@ -1520,21 +1507,21 @@
       <c r="E11" t="s">
         <v>38</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>8</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>6.7</v>
       </c>
       <c r="D12" t="s">
@@ -1543,21 +1530,21 @@
       <c r="E12" t="s">
         <v>41</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>15</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>25.9</v>
       </c>
       <c r="D13" t="s">
@@ -1566,18 +1553,18 @@
       <c r="E13" t="s">
         <v>44</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>45</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>32</v>
       </c>
       <c r="D14" t="s">
@@ -1586,18 +1573,18 @@
       <c r="E14" t="s">
         <v>47</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>48</v>
       </c>
       <c r="B15" t="s">
         <v>49</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>11.1</v>
       </c>
       <c r="D15" t="s">
@@ -1606,24 +1593,24 @@
       <c r="E15" t="s">
         <v>51</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>16</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>6</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>52</v>
       </c>
       <c r="B16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>63.6</v>
       </c>
       <c r="D16" t="s">
@@ -1632,21 +1619,21 @@
       <c r="E16" t="s">
         <v>54</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>1</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H16">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>56</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>47.8</v>
       </c>
       <c r="D17" t="s">
@@ -1655,18 +1642,18 @@
       <c r="E17" t="s">
         <v>58</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H17">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>59</v>
       </c>
       <c r="B18" t="s">
         <v>56</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>48.1</v>
       </c>
       <c r="D18" t="s">
@@ -1675,21 +1662,21 @@
       <c r="E18" t="s">
         <v>61</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18">
         <v>1</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>62</v>
       </c>
       <c r="B19" t="s">
         <v>56</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19">
         <v>51.9</v>
       </c>
       <c r="D19" t="s">
@@ -1698,18 +1685,18 @@
       <c r="E19" t="s">
         <v>64</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>65</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>38.1</v>
       </c>
       <c r="D20" t="s">
@@ -1718,18 +1705,18 @@
       <c r="E20" t="s">
         <v>67</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>68</v>
       </c>
       <c r="B21" t="s">
         <v>69</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>29.4</v>
       </c>
       <c r="D21" t="s">
@@ -1738,24 +1725,24 @@
       <c r="E21" t="s">
         <v>71</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21">
         <v>1</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21">
         <v>1</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H21">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>72</v>
       </c>
       <c r="B22" t="s">
         <v>69</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>6.2</v>
       </c>
       <c r="D22" t="s">
@@ -1764,18 +1751,18 @@
       <c r="E22" t="s">
         <v>74</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
       <c r="B23" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23">
         <v>55</v>
       </c>
       <c r="D23" t="s">
@@ -1784,22 +1771,22 @@
       <c r="E23" t="s">
         <v>77</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23">
         <v>2</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H23">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>78</v>
       </c>
       <c r="B24" t="s">
         <v>69</v>
       </c>
-      <c r="C24" t="n">
-        <v>90.90000000000001</v>
+      <c r="C24">
+        <v>90.9</v>
       </c>
       <c r="D24" t="s">
         <v>79</v>
@@ -1807,18 +1794,18 @@
       <c r="E24" t="s">
         <v>80</v>
       </c>
-      <c r="H24" t="n">
+      <c r="H24">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>81</v>
       </c>
       <c r="B25" t="s">
         <v>69</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25">
         <v>66.7</v>
       </c>
       <c r="D25" t="s">
@@ -1827,18 +1814,18 @@
       <c r="E25" t="s">
         <v>83</v>
       </c>
-      <c r="H25" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="H25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>84</v>
       </c>
       <c r="B26" t="s">
         <v>69</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26">
         <v>81.8</v>
       </c>
       <c r="D26" t="s">
@@ -1847,18 +1834,18 @@
       <c r="E26" t="s">
         <v>86</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H26">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>87</v>
       </c>
       <c r="B27" t="s">
         <v>88</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>41.2</v>
       </c>
       <c r="D27" t="s">
@@ -1867,18 +1854,18 @@
       <c r="E27" t="s">
         <v>90</v>
       </c>
-      <c r="H27" t="n">
+      <c r="H27">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>91</v>
       </c>
       <c r="B28" t="s">
         <v>88</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28">
         <v>65.5</v>
       </c>
       <c r="D28" t="s">
@@ -1887,24 +1874,24 @@
       <c r="E28" t="s">
         <v>93</v>
       </c>
-      <c r="F28" t="n">
+      <c r="F28">
         <v>1</v>
       </c>
-      <c r="G28" t="n">
+      <c r="G28">
         <v>1</v>
       </c>
-      <c r="H28" t="n">
+      <c r="H28">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>94</v>
       </c>
       <c r="B29" t="s">
         <v>88</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29">
         <v>44.8</v>
       </c>
       <c r="D29" t="s">
@@ -1913,18 +1900,18 @@
       <c r="E29" t="s">
         <v>96</v>
       </c>
-      <c r="H29" t="n">
+      <c r="H29">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>97</v>
       </c>
       <c r="B30" t="s">
         <v>88</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30">
         <v>32.1</v>
       </c>
       <c r="D30" t="s">
@@ -1933,18 +1920,18 @@
       <c r="E30" t="s">
         <v>99</v>
       </c>
-      <c r="H30" t="n">
+      <c r="H30">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>100</v>
       </c>
       <c r="B31" t="s">
         <v>88</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31">
         <v>15.4</v>
       </c>
       <c r="D31" t="s">
@@ -1953,18 +1940,18 @@
       <c r="E31" t="s">
         <v>102</v>
       </c>
-      <c r="H31" t="n">
+      <c r="H31">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>103</v>
       </c>
       <c r="B32" t="s">
         <v>88</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32">
         <v>45.5</v>
       </c>
       <c r="D32" t="s">
@@ -1973,18 +1960,18 @@
       <c r="E32" t="s">
         <v>105</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H32">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>106</v>
       </c>
       <c r="B33" t="s">
         <v>88</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33">
         <v>77.3</v>
       </c>
       <c r="D33" t="s">
@@ -1993,18 +1980,18 @@
       <c r="E33" t="s">
         <v>108</v>
       </c>
-      <c r="H33" t="n">
+      <c r="H33">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>109</v>
       </c>
       <c r="B34" t="s">
         <v>88</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34">
         <v>72.2</v>
       </c>
       <c r="D34" t="s">
@@ -2013,18 +2000,18 @@
       <c r="E34" t="s">
         <v>110</v>
       </c>
-      <c r="H34" t="n">
+      <c r="H34">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>111</v>
       </c>
       <c r="B35" t="s">
         <v>88</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35">
         <v>94.7</v>
       </c>
       <c r="D35" t="s">
@@ -2033,18 +2020,18 @@
       <c r="E35" t="s">
         <v>113</v>
       </c>
-      <c r="H35" t="n">
+      <c r="H35">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>114</v>
       </c>
       <c r="B36" t="s">
         <v>88</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36">
         <v>40</v>
       </c>
       <c r="D36" t="s">
@@ -2053,57 +2040,29 @@
       <c r="E36" t="s">
         <v>116</v>
       </c>
-      <c r="H36" t="n">
+      <c r="H36">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="D37" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="D38" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="D39" t="s">
-        <v>121</v>
-      </c>
-      <c r="E39" t="s">
-        <v>122</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="11.33203125"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:8">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2129,7 +2088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2137,22 +2096,22 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" t="n">
+        <v>119</v>
+      </c>
+      <c r="F2">
         <v>3</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2160,25 +2119,25 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E3" t="s">
         <v>44</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2186,22 +2145,22 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F4" t="n">
+        <v>124</v>
+      </c>
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2209,22 +2168,22 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" t="n">
+        <v>127</v>
+      </c>
+      <c r="F5">
         <v>5</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2232,25 +2191,25 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" t="n">
+        <v>130</v>
+      </c>
+      <c r="F6">
         <v>7</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2258,25 +2217,25 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" t="n">
+        <v>132</v>
+      </c>
+      <c r="F7">
         <v>5</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>4</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2284,22 +2243,22 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E8" t="s">
-        <v>140</v>
-      </c>
-      <c r="F8" t="n">
+        <v>135</v>
+      </c>
+      <c r="F8">
         <v>3</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2307,25 +2266,25 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E9" t="s">
-        <v>143</v>
-      </c>
-      <c r="F9" t="n">
+        <v>138</v>
+      </c>
+      <c r="F9">
         <v>13</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>2</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -2333,25 +2292,25 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
-      </c>
-      <c r="F10" t="n">
+        <v>141</v>
+      </c>
+      <c r="F10">
         <v>16</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>2</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -2359,22 +2318,22 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E11" t="s">
-        <v>149</v>
-      </c>
-      <c r="F11" t="n">
+        <v>144</v>
+      </c>
+      <c r="F11">
         <v>4</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -2382,25 +2341,25 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D12" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
-      </c>
-      <c r="F12" t="n">
+        <v>147</v>
+      </c>
+      <c r="F12">
         <v>11</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -2408,19 +2367,19 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
-      </c>
-      <c r="H13" t="n">
+        <v>150</v>
+      </c>
+      <c r="H13">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2428,22 +2387,22 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>156</v>
-      </c>
-      <c r="F14" t="n">
+        <v>151</v>
+      </c>
+      <c r="F14">
         <v>1</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -2451,25 +2410,25 @@
         <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D15" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E15" t="s">
-        <v>159</v>
-      </c>
-      <c r="F15" t="n">
+        <v>154</v>
+      </c>
+      <c r="F15">
         <v>11</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>4</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -2477,19 +2436,19 @@
         <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D16" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E16" t="s">
-        <v>162</v>
-      </c>
-      <c r="H16" t="n">
+        <v>157</v>
+      </c>
+      <c r="H16">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -2497,19 +2456,19 @@
         <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E17" t="s">
-        <v>165</v>
-      </c>
-      <c r="H17" t="n">
+        <v>160</v>
+      </c>
+      <c r="H17">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -2517,19 +2476,19 @@
         <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D18" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E18" t="s">
-        <v>168</v>
-      </c>
-      <c r="H18" t="n">
+        <v>163</v>
+      </c>
+      <c r="H18">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -2537,19 +2496,19 @@
         <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D19" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E19" t="s">
-        <v>129</v>
-      </c>
-      <c r="H19" t="n">
+        <v>124</v>
+      </c>
+      <c r="H19">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -2557,19 +2516,19 @@
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E20" t="s">
-        <v>173</v>
-      </c>
-      <c r="H20" t="n">
+        <v>168</v>
+      </c>
+      <c r="H20">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -2577,22 +2536,22 @@
         <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E21" t="s">
-        <v>176</v>
-      </c>
-      <c r="F21" t="n">
+        <v>171</v>
+      </c>
+      <c r="F21">
         <v>1</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H21">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2600,22 +2559,22 @@
         <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>178</v>
-      </c>
-      <c r="F22" t="n">
+        <v>173</v>
+      </c>
+      <c r="F22">
         <v>1</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -2623,22 +2582,22 @@
         <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D23" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E23" t="s">
-        <v>181</v>
-      </c>
-      <c r="F23" t="n">
+        <v>176</v>
+      </c>
+      <c r="F23">
         <v>1</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H23">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -2646,19 +2605,19 @@
         <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D24" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E24" t="s">
-        <v>184</v>
-      </c>
-      <c r="H24" t="n">
+        <v>179</v>
+      </c>
+      <c r="H24">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -2666,19 +2625,19 @@
         <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D25" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E25" t="s">
-        <v>187</v>
-      </c>
-      <c r="H25" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>182</v>
+      </c>
+      <c r="H25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -2686,19 +2645,19 @@
         <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D26" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E26" t="s">
-        <v>190</v>
-      </c>
-      <c r="H26" t="n">
+        <v>185</v>
+      </c>
+      <c r="H26">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -2706,19 +2665,19 @@
         <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>192</v>
-      </c>
-      <c r="H27" t="n">
+        <v>187</v>
+      </c>
+      <c r="H27">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>91</v>
       </c>
@@ -2726,19 +2685,19 @@
         <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D28" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E28" t="s">
-        <v>195</v>
-      </c>
-      <c r="H28" t="n">
+        <v>190</v>
+      </c>
+      <c r="H28">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -2746,19 +2705,19 @@
         <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>196</v>
-      </c>
-      <c r="H29" t="n">
+        <v>191</v>
+      </c>
+      <c r="H29">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -2766,19 +2725,19 @@
         <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D30" t="s">
         <v>95</v>
       </c>
       <c r="E30" t="s">
-        <v>198</v>
-      </c>
-      <c r="H30" t="n">
+        <v>193</v>
+      </c>
+      <c r="H30">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>100</v>
       </c>
@@ -2786,19 +2745,19 @@
         <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D31" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E31" t="s">
-        <v>201</v>
-      </c>
-      <c r="H31" t="n">
+        <v>196</v>
+      </c>
+      <c r="H31">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -2806,19 +2765,19 @@
         <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D32" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E32" t="s">
-        <v>203</v>
-      </c>
-      <c r="H32" t="n">
+        <v>198</v>
+      </c>
+      <c r="H32">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -2826,19 +2785,19 @@
         <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D33" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E33" t="s">
-        <v>206</v>
-      </c>
-      <c r="H33" t="n">
+        <v>201</v>
+      </c>
+      <c r="H33">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -2846,19 +2805,19 @@
         <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D34" t="s">
         <v>23</v>
       </c>
       <c r="E34" t="s">
-        <v>208</v>
-      </c>
-      <c r="H34" t="n">
+        <v>203</v>
+      </c>
+      <c r="H34">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>111</v>
       </c>
@@ -2866,19 +2825,19 @@
         <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D35" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E35" t="s">
-        <v>211</v>
-      </c>
-      <c r="H35" t="n">
+        <v>206</v>
+      </c>
+      <c r="H35">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>114</v>
       </c>
@@ -2886,62 +2845,34 @@
         <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D36" t="s">
         <v>101</v>
       </c>
       <c r="E36" t="s">
-        <v>213</v>
-      </c>
-      <c r="H36" t="n">
+        <v>208</v>
+      </c>
+      <c r="H36">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="D37" t="s">
-        <v>214</v>
-      </c>
-      <c r="E37" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="D38" t="s">
-        <v>216</v>
-      </c>
-      <c r="E38" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="D39" t="s">
-        <v>121</v>
-      </c>
-      <c r="E39" t="s">
-        <v>218</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:8">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2967,7 +2898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2975,25 +2906,25 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="E2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F2" t="n">
+        <v>211</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3001,22 +2932,22 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D3" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F3" t="n">
+        <v>214</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -3024,22 +2955,22 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E4" t="s">
-        <v>226</v>
-      </c>
-      <c r="F4" t="n">
+        <v>217</v>
+      </c>
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3047,25 +2978,25 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="D5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E5" t="s">
-        <v>229</v>
-      </c>
-      <c r="F5" t="n">
+        <v>220</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>2</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3073,25 +3004,25 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D6" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
-      </c>
-      <c r="F6" t="n">
+        <v>179</v>
+      </c>
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -3099,25 +3030,25 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D7" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E7" t="s">
-        <v>234</v>
-      </c>
-      <c r="F7" t="n">
+        <v>225</v>
+      </c>
+      <c r="F7">
         <v>5</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>2</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -3125,19 +3056,19 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D8" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E8" t="s">
-        <v>236</v>
-      </c>
-      <c r="H8" t="n">
+        <v>227</v>
+      </c>
+      <c r="H8">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -3145,22 +3076,22 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D9" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="E9" t="s">
-        <v>238</v>
-      </c>
-      <c r="F9" t="n">
+        <v>229</v>
+      </c>
+      <c r="F9">
         <v>1</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -3168,22 +3099,22 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D10" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="E10" t="s">
-        <v>241</v>
-      </c>
-      <c r="F10" t="n">
+        <v>232</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -3191,22 +3122,22 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E11" t="s">
-        <v>243</v>
-      </c>
-      <c r="F11" t="n">
+        <v>234</v>
+      </c>
+      <c r="F11">
         <v>1</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -3214,22 +3145,22 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="D12" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="E12" t="s">
-        <v>246</v>
-      </c>
-      <c r="F12" t="n">
+        <v>237</v>
+      </c>
+      <c r="F12">
         <v>3</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -3237,19 +3168,19 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="D13" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="E13" t="s">
         <v>61</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -3257,22 +3188,22 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="D14" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F14" t="n">
+        <v>137</v>
+      </c>
+      <c r="F14">
         <v>1</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -3280,25 +3211,25 @@
         <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D15" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E15" t="s">
-        <v>249</v>
-      </c>
-      <c r="F15" t="n">
+        <v>240</v>
+      </c>
+      <c r="F15">
         <v>6</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>2</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -3306,19 +3237,19 @@
         <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D16" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="E16" t="s">
-        <v>251</v>
-      </c>
-      <c r="H16" t="n">
+        <v>242</v>
+      </c>
+      <c r="H16">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -3326,19 +3257,19 @@
         <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="D17" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="E17" t="s">
-        <v>253</v>
-      </c>
-      <c r="H17" t="n">
+        <v>244</v>
+      </c>
+      <c r="H17">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -3346,19 +3277,19 @@
         <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="D18" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="E18" t="s">
-        <v>256</v>
-      </c>
-      <c r="H18" t="n">
+        <v>247</v>
+      </c>
+      <c r="H18">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3366,19 +3297,19 @@
         <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="D19" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="E19" t="s">
         <v>23</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -3386,19 +3317,19 @@
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="D20" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E20" t="s">
-        <v>261</v>
-      </c>
-      <c r="H20" t="n">
+        <v>252</v>
+      </c>
+      <c r="H20">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -3406,19 +3337,19 @@
         <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="D21" t="s">
         <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>263</v>
-      </c>
-      <c r="H21" t="n">
+        <v>254</v>
+      </c>
+      <c r="H21">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -3426,22 +3357,22 @@
         <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D22" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="E22" t="s">
-        <v>266</v>
-      </c>
-      <c r="F22" t="n">
+        <v>257</v>
+      </c>
+      <c r="F22">
         <v>1</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -3449,22 +3380,22 @@
         <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="D23" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E23" t="s">
-        <v>269</v>
-      </c>
-      <c r="F23" t="n">
+        <v>260</v>
+      </c>
+      <c r="F23">
         <v>1</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H23">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -3472,19 +3403,19 @@
         <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D24" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="E24" t="s">
-        <v>271</v>
-      </c>
-      <c r="H24" t="n">
+        <v>262</v>
+      </c>
+      <c r="H24">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -3492,19 +3423,19 @@
         <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D25" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="E25" t="s">
-        <v>273</v>
-      </c>
-      <c r="H25" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>264</v>
+      </c>
+      <c r="H25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -3512,19 +3443,19 @@
         <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>274</v>
-      </c>
-      <c r="H26" t="n">
+        <v>265</v>
+      </c>
+      <c r="H26">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -3532,19 +3463,19 @@
         <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="D27" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="E27" t="s">
-        <v>276</v>
-      </c>
-      <c r="H27" t="n">
+        <v>267</v>
+      </c>
+      <c r="H27">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>91</v>
       </c>
@@ -3552,19 +3483,19 @@
         <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="D28" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="E28" t="s">
-        <v>279</v>
-      </c>
-      <c r="H28" t="n">
+        <v>270</v>
+      </c>
+      <c r="H28">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -3572,19 +3503,19 @@
         <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="D29" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="E29" t="s">
-        <v>282</v>
-      </c>
-      <c r="H29" t="n">
+        <v>273</v>
+      </c>
+      <c r="H29">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -3592,19 +3523,19 @@
         <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D30" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="E30" t="s">
-        <v>284</v>
-      </c>
-      <c r="H30" t="n">
+        <v>275</v>
+      </c>
+      <c r="H30">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>100</v>
       </c>
@@ -3612,19 +3543,19 @@
         <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D31" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="E31" t="s">
-        <v>287</v>
-      </c>
-      <c r="H31" t="n">
+        <v>278</v>
+      </c>
+      <c r="H31">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>103</v>
       </c>
@@ -3632,19 +3563,19 @@
         <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D32" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="E32" t="s">
         <v>98</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H32">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -3652,19 +3583,19 @@
         <v>88</v>
       </c>
       <c r="C33" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="D33" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="E33" t="s">
-        <v>291</v>
-      </c>
-      <c r="H33" t="n">
+        <v>282</v>
+      </c>
+      <c r="H33">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -3672,19 +3603,19 @@
         <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D34" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="E34" t="s">
-        <v>293</v>
-      </c>
-      <c r="H34" t="n">
+        <v>284</v>
+      </c>
+      <c r="H34">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>111</v>
       </c>
@@ -3692,19 +3623,19 @@
         <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D35" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="E35" t="s">
-        <v>295</v>
-      </c>
-      <c r="H35" t="n">
+        <v>286</v>
+      </c>
+      <c r="H35">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>114</v>
       </c>
@@ -3712,79 +3643,79 @@
         <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D36" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="E36" t="s">
-        <v>297</v>
-      </c>
-      <c r="H36" t="n">
+        <v>288</v>
+      </c>
+      <c r="H36">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B37" t="s">
         <v>88</v>
       </c>
       <c r="C37" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D37" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E37" t="s">
-        <v>300</v>
-      </c>
-      <c r="H37" t="n">
+        <v>291</v>
+      </c>
+      <c r="H37">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B38" t="s">
         <v>88</v>
       </c>
       <c r="C38" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D38" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="E38" t="s">
-        <v>304</v>
-      </c>
-      <c r="H38" t="n">
+        <v>295</v>
+      </c>
+      <c r="H38">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B39" t="s">
         <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D39" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E39" t="s">
-        <v>306</v>
-      </c>
-      <c r="H39" t="n">
+        <v>297</v>
+      </c>
+      <c r="H39">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>